<commit_message>
Playing with Pandas from 6/13/19
</commit_message>
<xml_diff>
--- a/Mod_1/Pandas/grades.xlsx
+++ b/Mod_1/Pandas/grades.xlsx
@@ -429,16 +429,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E2">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F2">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -449,16 +449,16 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>87</v>
       </c>
       <c r="E3">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F3">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -469,16 +469,16 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -489,16 +489,16 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D5">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E5">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F5">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>